<commit_message>
Wrote Backplane Design Document
</commit_message>
<xml_diff>
--- a/CougSat1-Backplane/Documentation/Native/ElectricalBusAllocation.xlsx
+++ b/CougSat1-Backplane/Documentation/Native/ElectricalBusAllocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1-Backplane\Documentation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A2E13C-5D80-4496-A111-0601D10FACB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14474438-3FE4-40FD-A374-45D332B86FD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>BUS_JTAG_TMS</t>
-  </si>
-  <si>
-    <t>Shared JTAG interface for subsystem  software update via IHU. Max 1 device at a time, normally disconnected</t>
   </si>
   <si>
     <t>BUS_I2C1_SDA</t>
@@ -177,9 +174,6 @@
     <t>SPI_EN_CAM0</t>
   </si>
   <si>
-    <t>JTAG_SEL_RCS</t>
-  </si>
-  <si>
     <t>Ctrl</t>
   </si>
   <si>
@@ -538,9 +532,6 @@
     <t>GPIO-9</t>
   </si>
   <si>
-    <t>Shared JTAG interface for subsystem  software update via IHU. Max 1 device at a time, normally high impedance</t>
-  </si>
-  <si>
     <t>81, 83</t>
   </si>
   <si>
@@ -584,6 +575,15 @@
   </si>
   <si>
     <t>Serial interface for dedicated communication with the Comms</t>
+  </si>
+  <si>
+    <t>JTAG_SEL_COMMS</t>
+  </si>
+  <si>
+    <t>Shared JTAG interface for subsystem software update via IFJR. Max 1 device at a time, normally high impedance</t>
+  </si>
+  <si>
+    <t>Shared JTAG interface for subsystem software update via IFJR. Max 1 device at a time, normally disconnected</t>
   </si>
 </sst>
 </file>
@@ -983,17 +983,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1004,29 +1022,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1371,7 +1371,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="62"/>
       <c r="C3" s="62"/>
@@ -1444,9 +1444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39:D42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,10 +1459,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>2</v>
@@ -1473,437 +1473,437 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="52" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="52" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="53" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="67"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="67"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" s="67"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="67"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
       <c r="B30" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="45"/>
       <c r="B31" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="64"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="65"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D35" s="63" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D36" s="64"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D37" s="64"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D38" s="65"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="68" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>5</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>6</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>8</v>
@@ -1930,133 +1930,133 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
       <c r="B46" s="56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C46" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D46" s="36"/>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C47" s="57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C48" s="57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="58" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C49" s="57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="58" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C50" s="57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="58" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C51" s="57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="58" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C52" s="57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C53" s="57" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C54" s="57" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C55" s="57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17"/>
       <c r="B56" s="28" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C56" s="59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D56" s="38"/>
     </row>
@@ -2081,9 +2081,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76:A81"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,11 +2114,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="72" t="s">
-        <v>39</v>
+      <c r="A2" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="31">
         <v>1</v>
@@ -2126,31 +2126,31 @@
       <c r="D2" s="31">
         <v>2</v>
       </c>
-      <c r="E2" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="82" t="s">
-        <v>65</v>
+      <c r="E2" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="74"/>
       <c r="C3" s="31">
         <v>3</v>
       </c>
       <c r="D3" s="31">
         <v>4</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="83"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="71"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="72" t="s">
-        <v>40</v>
+      <c r="A4" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="31">
         <v>5</v>
@@ -2158,31 +2158,31 @@
       <c r="D4" s="50">
         <v>6</v>
       </c>
-      <c r="E4" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="82" t="s">
-        <v>66</v>
+      <c r="E4" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="31">
         <v>7</v>
       </c>
       <c r="D5" s="50">
         <v>8</v>
       </c>
-      <c r="E5" s="69"/>
-      <c r="F5" s="83"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>41</v>
+      <c r="A6" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>39</v>
       </c>
       <c r="C6" s="31">
         <v>9</v>
@@ -2190,31 +2190,31 @@
       <c r="D6" s="50">
         <v>10</v>
       </c>
-      <c r="E6" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="82" t="s">
-        <v>67</v>
+      <c r="E6" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="31">
         <v>11</v>
       </c>
       <c r="D7" s="50">
         <v>12</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="83"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="71"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="72" t="s">
-        <v>42</v>
+      <c r="A8" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>40</v>
       </c>
       <c r="C8" s="31">
         <v>13</v>
@@ -2222,31 +2222,31 @@
       <c r="D8" s="50">
         <v>14</v>
       </c>
-      <c r="E8" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="82" t="s">
-        <v>68</v>
+      <c r="E8" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="31">
         <v>15</v>
       </c>
       <c r="D9" s="50">
         <v>16</v>
       </c>
-      <c r="E9" s="69"/>
-      <c r="F9" s="83"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="72" t="s">
-        <v>43</v>
+      <c r="A10" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="31">
         <v>17</v>
@@ -2254,31 +2254,31 @@
       <c r="D10" s="50">
         <v>18</v>
       </c>
-      <c r="E10" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="82" t="s">
-        <v>69</v>
+      <c r="E10" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="70" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="31">
         <v>19</v>
       </c>
       <c r="D11" s="50">
         <v>20</v>
       </c>
-      <c r="E11" s="69"/>
-      <c r="F11" s="83"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="71"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="72" t="s">
-        <v>44</v>
+      <c r="A12" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>42</v>
       </c>
       <c r="C12" s="31">
         <v>21</v>
@@ -2286,31 +2286,31 @@
       <c r="D12" s="50">
         <v>22</v>
       </c>
-      <c r="E12" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="82" t="s">
-        <v>70</v>
+      <c r="E12" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="72"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="31">
         <v>23</v>
       </c>
       <c r="D13" s="50">
         <v>24</v>
       </c>
-      <c r="E13" s="69"/>
-      <c r="F13" s="83"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="71"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="72" t="s">
-        <v>45</v>
+      <c r="A14" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>43</v>
       </c>
       <c r="C14" s="31">
         <v>25</v>
@@ -2318,31 +2318,31 @@
       <c r="D14" s="50">
         <v>26</v>
       </c>
-      <c r="E14" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="82" t="s">
-        <v>71</v>
+      <c r="E14" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="70" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="31">
         <v>27</v>
       </c>
       <c r="D15" s="50">
         <v>28</v>
       </c>
-      <c r="E15" s="69"/>
-      <c r="F15" s="83"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="71"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="72" t="s">
-        <v>46</v>
+      <c r="A16" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>44</v>
       </c>
       <c r="C16" s="31">
         <v>29</v>
@@ -2350,31 +2350,31 @@
       <c r="D16" s="50">
         <v>30</v>
       </c>
-      <c r="E16" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="82" t="s">
-        <v>72</v>
+      <c r="E16" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="70" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="72"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="31">
         <v>31</v>
       </c>
       <c r="D17" s="50">
         <v>32</v>
       </c>
-      <c r="E17" s="69"/>
-      <c r="F17" s="83"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="71"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="72" t="s">
-        <v>47</v>
+      <c r="A18" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="31">
         <v>33</v>
@@ -2382,31 +2382,31 @@
       <c r="D18" s="50">
         <v>34</v>
       </c>
-      <c r="E18" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="82" t="s">
-        <v>73</v>
+      <c r="E18" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="70" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="72"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="31">
         <v>35</v>
       </c>
       <c r="D19" s="50">
         <v>36</v>
       </c>
-      <c r="E19" s="69"/>
-      <c r="F19" s="83"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="71"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="72" t="s">
-        <v>48</v>
+      <c r="A20" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>46</v>
       </c>
       <c r="C20" s="31">
         <v>37</v>
@@ -2414,31 +2414,31 @@
       <c r="D20" s="50">
         <v>38</v>
       </c>
-      <c r="E20" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="82" t="s">
-        <v>74</v>
+      <c r="E20" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="70" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="31">
         <v>39</v>
       </c>
       <c r="D21" s="50">
         <v>40</v>
       </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="83"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="71"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="72" t="s">
-        <v>49</v>
+      <c r="A22" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>47</v>
       </c>
       <c r="C22" s="31">
         <v>41</v>
@@ -2446,33 +2446,33 @@
       <c r="D22" s="50">
         <v>42</v>
       </c>
-      <c r="E22" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="82" t="s">
-        <v>75</v>
+      <c r="E22" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="70" t="s">
+        <v>73</v>
       </c>
       <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="31">
         <v>43</v>
       </c>
       <c r="D23" s="50">
         <v>44</v>
       </c>
-      <c r="E23" s="69"/>
-      <c r="F23" s="83"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="71"/>
       <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="70" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="72" t="s">
-        <v>50</v>
+      <c r="A24" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>48</v>
       </c>
       <c r="C24" s="31">
         <v>45</v>
@@ -2480,33 +2480,33 @@
       <c r="D24" s="50">
         <v>46</v>
       </c>
-      <c r="E24" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="82" t="s">
-        <v>76</v>
+      <c r="E24" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="70" t="s">
+        <v>74</v>
       </c>
       <c r="G24" s="33"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="31">
         <v>47</v>
       </c>
       <c r="D25" s="50">
         <v>48</v>
       </c>
-      <c r="E25" s="69"/>
-      <c r="F25" s="83"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="71"/>
       <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="72" t="s">
-        <v>51</v>
+      <c r="A26" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="74" t="s">
+        <v>49</v>
       </c>
       <c r="C26" s="31">
         <v>49</v>
@@ -2514,33 +2514,33 @@
       <c r="D26" s="50">
         <v>50</v>
       </c>
-      <c r="E26" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="82" t="s">
-        <v>77</v>
+      <c r="E26" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="70" t="s">
+        <v>75</v>
       </c>
       <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="31">
         <v>51</v>
       </c>
       <c r="D27" s="50">
         <v>52</v>
       </c>
-      <c r="E27" s="69"/>
-      <c r="F27" s="83"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="72" t="s">
-        <v>52</v>
+      <c r="A28" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>50</v>
       </c>
       <c r="C28" s="32">
         <v>53</v>
@@ -2548,33 +2548,33 @@
       <c r="D28" s="51">
         <v>54</v>
       </c>
-      <c r="E28" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="82" t="s">
-        <v>78</v>
+      <c r="E28" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="70" t="s">
+        <v>76</v>
       </c>
       <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="71"/>
-      <c r="B29" s="72"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="32">
         <v>55</v>
       </c>
       <c r="D29" s="51">
         <v>56</v>
       </c>
-      <c r="E29" s="69"/>
-      <c r="F29" s="83"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="71"/>
       <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="70" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="72" t="s">
-        <v>53</v>
+      <c r="A30" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="74" t="s">
+        <v>51</v>
       </c>
       <c r="C30" s="32">
         <v>57</v>
@@ -2582,33 +2582,33 @@
       <c r="D30" s="51">
         <v>58</v>
       </c>
-      <c r="E30" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="82" t="s">
-        <v>79</v>
+      <c r="E30" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="70" t="s">
+        <v>77</v>
       </c>
       <c r="G30" s="33"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="32">
         <v>59</v>
       </c>
       <c r="D31" s="51">
         <v>60</v>
       </c>
-      <c r="E31" s="69"/>
-      <c r="F31" s="83"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="71"/>
       <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="72" t="s">
-        <v>54</v>
+      <c r="A32" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="74" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="32">
         <v>61</v>
@@ -2616,33 +2616,33 @@
       <c r="D32" s="51">
         <v>62</v>
       </c>
-      <c r="E32" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="F32" s="82" t="s">
-        <v>80</v>
+      <c r="E32" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="70" t="s">
+        <v>78</v>
       </c>
       <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="71"/>
-      <c r="B33" s="72"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="32">
         <v>63</v>
       </c>
       <c r="D33" s="51">
         <v>64</v>
       </c>
-      <c r="E33" s="69"/>
-      <c r="F33" s="83"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="71"/>
       <c r="G33" s="33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="72" t="s">
-        <v>55</v>
+      <c r="A34" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>53</v>
       </c>
       <c r="C34" s="32">
         <v>65</v>
@@ -2650,33 +2650,33 @@
       <c r="D34" s="51">
         <v>66</v>
       </c>
-      <c r="E34" s="69" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="82" t="s">
-        <v>81</v>
+      <c r="E34" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="70" t="s">
+        <v>79</v>
       </c>
       <c r="G34" s="33"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
-      <c r="B35" s="72"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="32">
         <v>67</v>
       </c>
       <c r="D35" s="51">
         <v>68</v>
       </c>
-      <c r="E35" s="69"/>
-      <c r="F35" s="83"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="71"/>
       <c r="G35" s="33"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="72" t="s">
-        <v>56</v>
+      <c r="A36" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="74" t="s">
+        <v>54</v>
       </c>
       <c r="C36" s="32">
         <v>69</v>
@@ -2684,33 +2684,33 @@
       <c r="D36" s="51">
         <v>70</v>
       </c>
-      <c r="E36" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="82" t="s">
-        <v>82</v>
+      <c r="E36" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="70" t="s">
+        <v>80</v>
       </c>
       <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
-      <c r="B37" s="72"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="74"/>
       <c r="C37" s="32">
         <v>71</v>
       </c>
       <c r="D37" s="51">
         <v>72</v>
       </c>
-      <c r="E37" s="69"/>
-      <c r="F37" s="83"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="71"/>
       <c r="G37" s="33"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="72" t="s">
-        <v>57</v>
+      <c r="A38" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>55</v>
       </c>
       <c r="C38" s="32">
         <v>73</v>
@@ -2718,33 +2718,33 @@
       <c r="D38" s="51">
         <v>74</v>
       </c>
-      <c r="E38" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="82" t="s">
-        <v>83</v>
+      <c r="E38" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="70" t="s">
+        <v>81</v>
       </c>
       <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="72"/>
+      <c r="A39" s="69"/>
+      <c r="B39" s="74"/>
       <c r="C39" s="32">
         <v>75</v>
       </c>
       <c r="D39" s="51">
         <v>76</v>
       </c>
-      <c r="E39" s="69"/>
-      <c r="F39" s="83"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="71"/>
       <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="72" t="s">
-        <v>58</v>
+      <c r="A40" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="74" t="s">
+        <v>56</v>
       </c>
       <c r="C40" s="32">
         <v>77</v>
@@ -2752,33 +2752,33 @@
       <c r="D40" s="51">
         <v>78</v>
       </c>
-      <c r="E40" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="82" t="s">
-        <v>84</v>
+      <c r="E40" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="70" t="s">
+        <v>82</v>
       </c>
       <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="71"/>
-      <c r="B41" s="72"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="74"/>
       <c r="C41" s="32">
         <v>79</v>
       </c>
       <c r="D41" s="51">
         <v>80</v>
       </c>
-      <c r="E41" s="69"/>
-      <c r="F41" s="83"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="71"/>
       <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="79" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="72" t="s">
-        <v>141</v>
+      <c r="A42" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>139</v>
       </c>
       <c r="C42" s="12">
         <v>81</v>
@@ -2786,33 +2786,33 @@
       <c r="D42" s="7">
         <v>82</v>
       </c>
-      <c r="E42" s="69" t="s">
-        <v>23</v>
+      <c r="E42" s="76" t="s">
+        <v>22</v>
       </c>
       <c r="F42" s="68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G42" s="33"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
-      <c r="B43" s="76"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="75"/>
       <c r="C43" s="12">
         <v>83</v>
       </c>
       <c r="D43" s="7">
         <v>84</v>
       </c>
-      <c r="E43" s="69"/>
+      <c r="E43" s="76"/>
       <c r="F43" s="68"/>
       <c r="G43" s="33"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="79" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="72" t="s">
-        <v>142</v>
+      <c r="A44" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="74" t="s">
+        <v>140</v>
       </c>
       <c r="C44" s="12">
         <v>85</v>
@@ -2820,27 +2820,27 @@
       <c r="D44" s="7">
         <v>86</v>
       </c>
-      <c r="E44" s="69"/>
+      <c r="E44" s="76"/>
       <c r="F44" s="68"/>
       <c r="G44" s="33"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="79"/>
-      <c r="B45" s="76"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="75"/>
       <c r="C45" s="12">
         <v>87</v>
       </c>
       <c r="D45" s="7">
         <v>88</v>
       </c>
-      <c r="E45" s="69"/>
+      <c r="E45" s="76"/>
       <c r="F45" s="68"/>
       <c r="G45" s="33"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="79"/>
-      <c r="B46" s="72" t="s">
-        <v>143</v>
+      <c r="A46" s="73"/>
+      <c r="B46" s="74" t="s">
+        <v>141</v>
       </c>
       <c r="C46" s="12">
         <v>89</v>
@@ -2848,27 +2848,27 @@
       <c r="D46" s="7">
         <v>90</v>
       </c>
-      <c r="E46" s="69"/>
+      <c r="E46" s="76"/>
       <c r="F46" s="68"/>
       <c r="G46" s="33"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="79"/>
-      <c r="B47" s="76"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="12">
         <v>91</v>
       </c>
       <c r="D47" s="7">
         <v>92</v>
       </c>
-      <c r="E47" s="69"/>
+      <c r="E47" s="76"/>
       <c r="F47" s="68"/>
       <c r="G47" s="33"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="79"/>
-      <c r="B48" s="72" t="s">
-        <v>144</v>
+      <c r="A48" s="73"/>
+      <c r="B48" s="74" t="s">
+        <v>142</v>
       </c>
       <c r="C48" s="12">
         <v>93</v>
@@ -2876,27 +2876,27 @@
       <c r="D48" s="7">
         <v>94</v>
       </c>
-      <c r="E48" s="69"/>
+      <c r="E48" s="76"/>
       <c r="F48" s="68"/>
       <c r="G48" s="33"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="79"/>
-      <c r="B49" s="76"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="75"/>
       <c r="C49" s="12">
         <v>95</v>
       </c>
       <c r="D49" s="7">
         <v>96</v>
       </c>
-      <c r="E49" s="69"/>
+      <c r="E49" s="76"/>
       <c r="F49" s="68"/>
       <c r="G49" s="33"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="79"/>
-      <c r="B50" s="72" t="s">
-        <v>145</v>
+      <c r="A50" s="73"/>
+      <c r="B50" s="74" t="s">
+        <v>143</v>
       </c>
       <c r="C50" s="12">
         <v>97</v>
@@ -2904,27 +2904,27 @@
       <c r="D50" s="7">
         <v>98</v>
       </c>
-      <c r="E50" s="69"/>
+      <c r="E50" s="76"/>
       <c r="F50" s="68"/>
       <c r="G50" s="33"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="79"/>
-      <c r="B51" s="76"/>
+      <c r="A51" s="73"/>
+      <c r="B51" s="75"/>
       <c r="C51" s="12">
         <v>99</v>
       </c>
       <c r="D51" s="7">
         <v>100</v>
       </c>
-      <c r="E51" s="69"/>
+      <c r="E51" s="76"/>
       <c r="F51" s="68"/>
       <c r="G51" s="33"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="79"/>
-      <c r="B52" s="72" t="s">
-        <v>146</v>
+      <c r="A52" s="73"/>
+      <c r="B52" s="74" t="s">
+        <v>144</v>
       </c>
       <c r="C52" s="12">
         <v>101</v>
@@ -2932,27 +2932,27 @@
       <c r="D52" s="7">
         <v>102</v>
       </c>
-      <c r="E52" s="69"/>
+      <c r="E52" s="76"/>
       <c r="F52" s="68"/>
       <c r="G52" s="33"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="79"/>
-      <c r="B53" s="76"/>
+      <c r="A53" s="73"/>
+      <c r="B53" s="75"/>
       <c r="C53" s="12">
         <v>103</v>
       </c>
       <c r="D53" s="7">
         <v>104</v>
       </c>
-      <c r="E53" s="69"/>
+      <c r="E53" s="76"/>
       <c r="F53" s="68"/>
       <c r="G53" s="33"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="79"/>
-      <c r="B54" s="72" t="s">
-        <v>147</v>
+      <c r="A54" s="73"/>
+      <c r="B54" s="74" t="s">
+        <v>145</v>
       </c>
       <c r="C54" s="12">
         <v>105</v>
@@ -2960,27 +2960,27 @@
       <c r="D54" s="7">
         <v>106</v>
       </c>
-      <c r="E54" s="69"/>
+      <c r="E54" s="76"/>
       <c r="F54" s="68"/>
       <c r="G54" s="33"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="79"/>
-      <c r="B55" s="76"/>
+      <c r="A55" s="73"/>
+      <c r="B55" s="75"/>
       <c r="C55" s="12">
         <v>107</v>
       </c>
       <c r="D55" s="7">
         <v>108</v>
       </c>
-      <c r="E55" s="69"/>
+      <c r="E55" s="76"/>
       <c r="F55" s="68"/>
       <c r="G55" s="33"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="79"/>
-      <c r="B56" s="72" t="s">
-        <v>148</v>
+      <c r="A56" s="73"/>
+      <c r="B56" s="74" t="s">
+        <v>146</v>
       </c>
       <c r="C56" s="12">
         <v>109</v>
@@ -2988,27 +2988,27 @@
       <c r="D56" s="7">
         <v>110</v>
       </c>
-      <c r="E56" s="69"/>
+      <c r="E56" s="76"/>
       <c r="F56" s="68"/>
       <c r="G56" s="33"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="79"/>
-      <c r="B57" s="76"/>
+      <c r="A57" s="73"/>
+      <c r="B57" s="75"/>
       <c r="C57" s="12">
         <v>111</v>
       </c>
       <c r="D57" s="7">
         <v>112</v>
       </c>
-      <c r="E57" s="69"/>
+      <c r="E57" s="76"/>
       <c r="F57" s="68"/>
       <c r="G57" s="33"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="71"/>
-      <c r="B58" s="72" t="s">
-        <v>149</v>
+      <c r="A58" s="69"/>
+      <c r="B58" s="74" t="s">
+        <v>147</v>
       </c>
       <c r="C58" s="12">
         <v>113</v>
@@ -3016,27 +3016,27 @@
       <c r="D58" s="7">
         <v>114</v>
       </c>
-      <c r="E58" s="69"/>
+      <c r="E58" s="76"/>
       <c r="F58" s="68"/>
       <c r="G58" s="33"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="71"/>
-      <c r="B59" s="76"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="75"/>
       <c r="C59" s="12">
         <v>115</v>
       </c>
       <c r="D59" s="7">
         <v>116</v>
       </c>
-      <c r="E59" s="69"/>
+      <c r="E59" s="76"/>
       <c r="F59" s="68"/>
       <c r="G59" s="33"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="71"/>
-      <c r="B60" s="72" t="s">
-        <v>150</v>
+      <c r="A60" s="69"/>
+      <c r="B60" s="74" t="s">
+        <v>148</v>
       </c>
       <c r="C60" s="12">
         <v>117</v>
@@ -3044,29 +3044,29 @@
       <c r="D60" s="7">
         <v>118</v>
       </c>
-      <c r="E60" s="69"/>
+      <c r="E60" s="76"/>
       <c r="F60" s="68"/>
       <c r="G60" s="33"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="71"/>
-      <c r="B61" s="76"/>
+      <c r="A61" s="69"/>
+      <c r="B61" s="75"/>
       <c r="C61" s="12">
         <v>119</v>
       </c>
       <c r="D61" s="7">
         <v>120</v>
       </c>
-      <c r="E61" s="69"/>
+      <c r="E61" s="76"/>
       <c r="F61" s="68"/>
       <c r="G61" s="33"/>
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="79" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="72" t="s">
-        <v>10</v>
+      <c r="A62" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="74" t="s">
+        <v>9</v>
       </c>
       <c r="C62" s="9">
         <v>121</v>
@@ -3074,27 +3074,27 @@
       <c r="D62" s="7">
         <v>122</v>
       </c>
-      <c r="E62" s="69"/>
+      <c r="E62" s="76"/>
       <c r="F62" s="68"/>
       <c r="G62" s="33"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="79"/>
-      <c r="B63" s="72"/>
+      <c r="A63" s="73"/>
+      <c r="B63" s="74"/>
       <c r="C63" s="9">
         <v>123</v>
       </c>
       <c r="D63" s="7">
         <v>124</v>
       </c>
-      <c r="E63" s="69"/>
+      <c r="E63" s="76"/>
       <c r="F63" s="68"/>
       <c r="G63" s="33"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="79"/>
-      <c r="B64" s="72" t="s">
-        <v>11</v>
+      <c r="A64" s="73"/>
+      <c r="B64" s="74" t="s">
+        <v>10</v>
       </c>
       <c r="C64" s="9">
         <v>125</v>
@@ -3102,27 +3102,27 @@
       <c r="D64" s="7">
         <v>126</v>
       </c>
-      <c r="E64" s="69"/>
+      <c r="E64" s="76"/>
       <c r="F64" s="68"/>
       <c r="G64" s="33"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="79"/>
-      <c r="B65" s="72"/>
+      <c r="A65" s="73"/>
+      <c r="B65" s="74"/>
       <c r="C65" s="9">
         <v>127</v>
       </c>
       <c r="D65" s="7">
         <v>128</v>
       </c>
-      <c r="E65" s="69"/>
+      <c r="E65" s="76"/>
       <c r="F65" s="68"/>
       <c r="G65" s="33"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="79"/>
-      <c r="B66" s="72" t="s">
-        <v>27</v>
+      <c r="A66" s="73"/>
+      <c r="B66" s="74" t="s">
+        <v>26</v>
       </c>
       <c r="C66" s="9">
         <v>129</v>
@@ -3130,29 +3130,29 @@
       <c r="D66" s="7">
         <v>130</v>
       </c>
-      <c r="E66" s="69"/>
+      <c r="E66" s="76"/>
       <c r="F66" s="68"/>
       <c r="G66" s="33"/>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="79"/>
-      <c r="B67" s="72"/>
+      <c r="A67" s="73"/>
+      <c r="B67" s="74"/>
       <c r="C67" s="9">
         <v>131</v>
       </c>
       <c r="D67" s="7">
         <v>132</v>
       </c>
-      <c r="E67" s="69"/>
+      <c r="E67" s="76"/>
       <c r="F67" s="68"/>
       <c r="G67" s="33"/>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="B68" s="73" t="s">
-        <v>162</v>
+      <c r="A68" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="79" t="s">
+        <v>159</v>
       </c>
       <c r="C68" s="10">
         <v>133</v>
@@ -3160,27 +3160,27 @@
       <c r="D68" s="7">
         <v>134</v>
       </c>
-      <c r="E68" s="69"/>
+      <c r="E68" s="76"/>
       <c r="F68" s="68"/>
       <c r="G68" s="33"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="75"/>
-      <c r="B69" s="73"/>
+      <c r="A69" s="81"/>
+      <c r="B69" s="79"/>
       <c r="C69" s="10">
         <v>135</v>
       </c>
       <c r="D69" s="7">
         <v>136</v>
       </c>
-      <c r="E69" s="69"/>
+      <c r="E69" s="76"/>
       <c r="F69" s="68"/>
       <c r="G69" s="33"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="75"/>
-      <c r="B70" s="73" t="s">
-        <v>163</v>
+      <c r="A70" s="81"/>
+      <c r="B70" s="79" t="s">
+        <v>160</v>
       </c>
       <c r="C70" s="10">
         <v>137</v>
@@ -3188,27 +3188,27 @@
       <c r="D70" s="7">
         <v>138</v>
       </c>
-      <c r="E70" s="69"/>
+      <c r="E70" s="76"/>
       <c r="F70" s="68"/>
       <c r="G70" s="33"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="75"/>
-      <c r="B71" s="73"/>
+      <c r="A71" s="81"/>
+      <c r="B71" s="79"/>
       <c r="C71" s="10">
         <v>139</v>
       </c>
       <c r="D71" s="7">
         <v>140</v>
       </c>
-      <c r="E71" s="69"/>
+      <c r="E71" s="76"/>
       <c r="F71" s="68"/>
       <c r="G71" s="33"/>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="75"/>
-      <c r="B72" s="73" t="s">
-        <v>164</v>
+      <c r="A72" s="81"/>
+      <c r="B72" s="79" t="s">
+        <v>161</v>
       </c>
       <c r="C72" s="10">
         <v>141</v>
@@ -3216,25 +3216,25 @@
       <c r="D72" s="7">
         <v>142</v>
       </c>
-      <c r="E72" s="69"/>
+      <c r="E72" s="76"/>
       <c r="F72" s="68"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="75"/>
-      <c r="B73" s="73"/>
+      <c r="A73" s="81"/>
+      <c r="B73" s="79"/>
       <c r="C73" s="10">
         <v>143</v>
       </c>
       <c r="D73" s="7">
         <v>144</v>
       </c>
-      <c r="E73" s="69"/>
+      <c r="E73" s="76"/>
       <c r="F73" s="68"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="75"/>
-      <c r="B74" s="73" t="s">
-        <v>165</v>
+      <c r="A74" s="81"/>
+      <c r="B74" s="79" t="s">
+        <v>162</v>
       </c>
       <c r="C74" s="10">
         <v>145</v>
@@ -3242,27 +3242,27 @@
       <c r="D74" s="7">
         <v>146</v>
       </c>
-      <c r="E74" s="69"/>
+      <c r="E74" s="76"/>
       <c r="F74" s="68"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="75"/>
-      <c r="B75" s="73"/>
+      <c r="A75" s="81"/>
+      <c r="B75" s="79"/>
       <c r="C75" s="10">
         <v>147</v>
       </c>
       <c r="D75" s="7">
         <v>148</v>
       </c>
-      <c r="E75" s="69"/>
+      <c r="E75" s="76"/>
       <c r="F75" s="68"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" s="72" t="s">
-        <v>30</v>
+      <c r="A76" s="82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="74" t="s">
+        <v>29</v>
       </c>
       <c r="C76" s="9">
         <v>149</v>
@@ -3270,25 +3270,25 @@
       <c r="D76" s="7">
         <v>150</v>
       </c>
-      <c r="E76" s="69"/>
+      <c r="E76" s="76"/>
       <c r="F76" s="68"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="77"/>
-      <c r="B77" s="72"/>
+      <c r="A77" s="82"/>
+      <c r="B77" s="74"/>
       <c r="C77" s="9">
         <v>151</v>
       </c>
       <c r="D77" s="7">
         <v>152</v>
       </c>
-      <c r="E77" s="69"/>
+      <c r="E77" s="76"/>
       <c r="F77" s="68"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="77"/>
-      <c r="B78" s="72" t="s">
-        <v>29</v>
+      <c r="A78" s="82"/>
+      <c r="B78" s="74" t="s">
+        <v>28</v>
       </c>
       <c r="C78" s="9">
         <v>153</v>
@@ -3296,25 +3296,25 @@
       <c r="D78" s="7">
         <v>154</v>
       </c>
-      <c r="E78" s="69"/>
+      <c r="E78" s="76"/>
       <c r="F78" s="68"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="77"/>
-      <c r="B79" s="72"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="74"/>
       <c r="C79" s="9">
         <v>155</v>
       </c>
       <c r="D79" s="7">
         <v>156</v>
       </c>
-      <c r="E79" s="69"/>
+      <c r="E79" s="76"/>
       <c r="F79" s="68"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="77"/>
-      <c r="B80" s="72" t="s">
-        <v>28</v>
+      <c r="A80" s="82"/>
+      <c r="B80" s="74" t="s">
+        <v>27</v>
       </c>
       <c r="C80" s="9">
         <v>157</v>
@@ -3322,27 +3322,27 @@
       <c r="D80" s="7">
         <v>158</v>
       </c>
-      <c r="E80" s="69"/>
+      <c r="E80" s="76"/>
       <c r="F80" s="68"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="77"/>
-      <c r="B81" s="72"/>
+      <c r="A81" s="82"/>
+      <c r="B81" s="74"/>
       <c r="C81" s="9">
         <v>159</v>
       </c>
       <c r="D81" s="7">
         <v>160</v>
       </c>
-      <c r="E81" s="69"/>
+      <c r="E81" s="76"/>
       <c r="F81" s="68"/>
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="B82" s="73" t="s">
+      <c r="A82" s="72" t="s">
         <v>32</v>
+      </c>
+      <c r="B82" s="79" t="s">
+        <v>31</v>
       </c>
       <c r="C82" s="11">
         <v>161</v>
@@ -3350,26 +3350,26 @@
       <c r="D82" s="7">
         <v>162</v>
       </c>
-      <c r="E82" s="69"/>
+      <c r="E82" s="76"/>
       <c r="F82" s="68"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="70"/>
-      <c r="B83" s="74"/>
+      <c r="A83" s="72"/>
+      <c r="B83" s="80"/>
       <c r="C83" s="11">
         <v>163</v>
       </c>
       <c r="D83" s="7">
         <v>164</v>
       </c>
-      <c r="E83" s="69"/>
+      <c r="E83" s="76"/>
       <c r="F83" s="68"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="B84" s="73" t="s">
+      <c r="A84" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" s="79" t="s">
         <v>3</v>
       </c>
       <c r="C84" s="9">
@@ -3378,26 +3378,26 @@
       <c r="D84" s="7">
         <v>166</v>
       </c>
-      <c r="E84" s="69"/>
+      <c r="E84" s="76"/>
       <c r="F84" s="68"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="77"/>
-      <c r="B85" s="74"/>
+      <c r="A85" s="82"/>
+      <c r="B85" s="80"/>
       <c r="C85" s="9">
         <v>167</v>
       </c>
       <c r="D85" s="7">
         <v>168</v>
       </c>
-      <c r="E85" s="69"/>
+      <c r="E85" s="76"/>
       <c r="F85" s="68"/>
     </row>
     <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" s="73" t="s">
+      <c r="A86" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C86" s="9">
@@ -3406,27 +3406,27 @@
       <c r="D86" s="7">
         <v>170</v>
       </c>
-      <c r="E86" s="69"/>
+      <c r="E86" s="76"/>
       <c r="F86" s="68"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="75"/>
-      <c r="B87" s="74"/>
+      <c r="A87" s="81"/>
+      <c r="B87" s="80"/>
       <c r="C87" s="9">
         <v>171</v>
       </c>
       <c r="D87" s="7">
         <v>172</v>
       </c>
-      <c r="E87" s="69"/>
+      <c r="E87" s="76"/>
       <c r="F87" s="68"/>
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="B88" s="72" t="s">
-        <v>13</v>
+      <c r="A88" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" s="74" t="s">
+        <v>12</v>
       </c>
       <c r="C88" s="9">
         <v>173</v>
@@ -3434,25 +3434,25 @@
       <c r="D88" s="7">
         <v>174</v>
       </c>
-      <c r="E88" s="69"/>
+      <c r="E88" s="76"/>
       <c r="F88" s="68"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="80"/>
-      <c r="B89" s="72"/>
+      <c r="A89" s="83"/>
+      <c r="B89" s="74"/>
       <c r="C89" s="9">
         <v>175</v>
       </c>
       <c r="D89" s="7">
         <v>176</v>
       </c>
-      <c r="E89" s="69"/>
+      <c r="E89" s="76"/>
       <c r="F89" s="68"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="80"/>
-      <c r="B90" s="72" t="s">
-        <v>12</v>
+      <c r="A90" s="83"/>
+      <c r="B90" s="74" t="s">
+        <v>11</v>
       </c>
       <c r="C90" s="9">
         <v>177</v>
@@ -3460,25 +3460,25 @@
       <c r="D90" s="7">
         <v>178</v>
       </c>
-      <c r="E90" s="69"/>
+      <c r="E90" s="76"/>
       <c r="F90" s="68"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="80"/>
-      <c r="B91" s="72"/>
+      <c r="A91" s="83"/>
+      <c r="B91" s="74"/>
       <c r="C91" s="9">
         <v>179</v>
       </c>
       <c r="D91" s="7">
         <v>180</v>
       </c>
-      <c r="E91" s="69"/>
+      <c r="E91" s="76"/>
       <c r="F91" s="68"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="80"/>
-      <c r="B92" s="72" t="s">
-        <v>26</v>
+      <c r="A92" s="83"/>
+      <c r="B92" s="74" t="s">
+        <v>25</v>
       </c>
       <c r="C92" s="9">
         <v>181</v>
@@ -3486,26 +3486,26 @@
       <c r="D92" s="7">
         <v>182</v>
       </c>
-      <c r="E92" s="69"/>
+      <c r="E92" s="76"/>
       <c r="F92" s="68"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="80"/>
-      <c r="B93" s="72"/>
+      <c r="A93" s="83"/>
+      <c r="B93" s="74"/>
       <c r="C93" s="9">
         <v>183</v>
       </c>
       <c r="D93" s="7">
         <v>184</v>
       </c>
-      <c r="E93" s="69"/>
+      <c r="E93" s="76"/>
       <c r="F93" s="68"/>
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="B94" s="73" t="s">
+      <c r="A94" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="79" t="s">
         <v>7</v>
       </c>
       <c r="C94" s="8">
@@ -3514,28 +3514,28 @@
       <c r="D94" s="8">
         <v>186</v>
       </c>
-      <c r="E94" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="F94" s="78" t="s">
-        <v>35</v>
+      <c r="E94" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="F94" s="77" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="70"/>
-      <c r="B95" s="73"/>
+      <c r="A95" s="72"/>
+      <c r="B95" s="79"/>
       <c r="C95" s="8">
         <v>187</v>
       </c>
       <c r="D95" s="8">
         <v>188</v>
       </c>
-      <c r="E95" s="78"/>
-      <c r="F95" s="78"/>
+      <c r="E95" s="77"/>
+      <c r="F95" s="77"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="70"/>
-      <c r="B96" s="73" t="s">
+      <c r="A96" s="72"/>
+      <c r="B96" s="79" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="8">
@@ -3544,28 +3544,28 @@
       <c r="D96" s="8">
         <v>190</v>
       </c>
-      <c r="E96" s="78" t="s">
-        <v>62</v>
-      </c>
-      <c r="F96" s="78" t="s">
+      <c r="E96" s="77" t="s">
         <v>60</v>
       </c>
+      <c r="F96" s="77" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="70"/>
-      <c r="B97" s="74"/>
+      <c r="A97" s="72"/>
+      <c r="B97" s="80"/>
       <c r="C97" s="8">
         <v>191</v>
       </c>
       <c r="D97" s="8">
         <v>192</v>
       </c>
-      <c r="E97" s="78"/>
-      <c r="F97" s="78"/>
+      <c r="E97" s="77"/>
+      <c r="F97" s="77"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="70"/>
-      <c r="B98" s="73" t="s">
+      <c r="A98" s="72"/>
+      <c r="B98" s="79" t="s">
         <v>6</v>
       </c>
       <c r="C98" s="8">
@@ -3574,26 +3574,26 @@
       <c r="D98" s="8">
         <v>194</v>
       </c>
-      <c r="E98" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="F98" s="81"/>
+      <c r="E98" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="F98" s="78"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="70"/>
-      <c r="B99" s="74"/>
+      <c r="A99" s="72"/>
+      <c r="B99" s="80"/>
       <c r="C99" s="8">
         <v>195</v>
       </c>
       <c r="D99" s="8">
         <v>196</v>
       </c>
-      <c r="E99" s="78"/>
-      <c r="F99" s="81"/>
+      <c r="E99" s="77"/>
+      <c r="F99" s="78"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="70"/>
-      <c r="B100" s="73" t="s">
+      <c r="A100" s="72"/>
+      <c r="B100" s="79" t="s">
         <v>8</v>
       </c>
       <c r="C100" s="8">
@@ -3602,22 +3602,22 @@
       <c r="D100" s="8">
         <v>198</v>
       </c>
-      <c r="E100" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="F100" s="78"/>
+      <c r="E100" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="F100" s="77"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="70"/>
-      <c r="B101" s="74"/>
+      <c r="A101" s="72"/>
+      <c r="B101" s="80"/>
       <c r="C101" s="8">
         <v>199</v>
       </c>
       <c r="D101" s="8">
         <v>200</v>
       </c>
-      <c r="E101" s="78"/>
-      <c r="F101" s="78"/>
+      <c r="E101" s="77"/>
+      <c r="F101" s="77"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" s="41"/>
@@ -3650,82 +3650,36 @@
     </row>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="E42:E93"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="F94:F95"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F42:F93"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A86:A87"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B70:B71"/>
@@ -3750,47 +3704,93 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="A28:A29"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
     <mergeCell ref="A94:A101"/>
     <mergeCell ref="B90:B91"/>
     <mergeCell ref="B88:B89"/>
     <mergeCell ref="B94:B95"/>
     <mergeCell ref="B86:B87"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="F94:F95"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F42:F93"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="E40:E41"/>
     <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A76:A81"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="E42:E93"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="3" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>